<commit_message>
changed input files to fix evp params
</commit_message>
<xml_diff>
--- a/scripts/__other__/__params__.xlsx
+++ b/scripts/__other__/__params__.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/moga_neml/scripts/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/moga_neml/scripts/__other__/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="223" documentId="13_ncr:1_{95957D69-0AFB-443E-BEFE-75031A2E559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C5C307F-8D72-422D-9B63-AEF2A89761BD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="40" windowWidth="14400" windowHeight="7270" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="3" r:id="rId1"/>
@@ -324,6 +324,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -857,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEDA563-F318-4852-865D-A2318D089824}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -2207,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283AF620-1FFC-4E74-9A03-F7E60FF34CC2}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="A10:C10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2977,6 +2981,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added script for initialising parameters
</commit_message>
<xml_diff>
--- a/scripts/__other__/__params__.xlsx
+++ b/scripts/__other__/__params__.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D52E2E-C802-4994-8F20-95FD09534868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE058509-C80F-4A10-A7C5-C1D9DEB5888D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="225" windowWidth="28515" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="1" r:id="rId1"/>
@@ -117,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -126,15 +126,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -419,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,25 +494,25 @@
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="1">
         <v>18.946000000000002</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="1">
         <v>109.11</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="1">
         <v>0.88795999999999997</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="1">
         <v>4.0578000000000003</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="1">
         <v>2454.9</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="1">
         <v>3.0287000000000001E-3</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="1">
         <v>9.1731000000000003E-6</v>
       </c>
     </row>
@@ -564,25 +555,25 @@
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="1">
         <v>35.813000000000002</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="1">
         <v>66.293999999999997</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="1">
         <v>1.5430999999999999</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="1">
         <v>2.4946000000000002</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="1">
         <v>20880</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="1">
         <v>3.3224000000000001E-3</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="1">
         <v>1.1038E-5</v>
       </c>
     </row>
@@ -625,25 +616,25 @@
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <v>14.122999999999999</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>22.803999999999998</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <v>3.7970999999999999</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="1">
         <v>2.9723999999999999</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>3710.4</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="1">
         <v>1.23E-2</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="1">
         <v>1.5129999999999999E-4</v>
       </c>
     </row>

</xml_diff>